<commit_message>
Added Automation coverage trend
</commit_message>
<xml_diff>
--- a/Polarion Quality Dashboard - example.xlsx
+++ b/Polarion Quality Dashboard - example.xlsx
@@ -4,9 +4,10 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="PQI Metrics" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Polarion test run" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Polarion test run by team" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Dashboard configuration" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Automation coverage" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Polarion test run" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="Polarion test run by team" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Dashboard configuration" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>Req coverage</t>
   </si>
@@ -911,11 +912,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="898464723"/>
-        <c:axId val="2106578324"/>
+        <c:axId val="717897760"/>
+        <c:axId val="475353037"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="898464723"/>
+        <c:axId val="717897760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,6 +944,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -960,10 +962,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2106578324"/>
+        <c:crossAx val="475353037"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106578324"/>
+        <c:axId val="475353037"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1034,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="898464723"/>
+        <c:crossAx val="717897760"/>
       </c:valAx>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -1048,6 +1050,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1076,16 +1079,17 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="390520533"/>
-        <c:axId val="1846299418"/>
+        <c:axId val="1888623446"/>
+        <c:axId val="281205483"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="390520533"/>
+        <c:axId val="1888623446"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -1103,10 +1107,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1846299418"/>
+        <c:crossAx val="281205483"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1846299418"/>
+        <c:axId val="281205483"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1179,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390520533"/>
+        <c:crossAx val="1888623446"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -1203,6 +1207,381 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Automation coverage'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4285F4"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Automation coverage'!$A$2:$A$19</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Automation coverage'!$B$2:$B$19</c:f>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Automation coverage'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F1C232"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Automation coverage'!$A$2:$A$19</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Automation coverage'!$C$2:$C$19</c:f>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Automation coverage'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C53929"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Automation coverage'!$A$2:$A$19</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Automation coverage'!$D$2:$D$19</c:f>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="169839447"/>
+        <c:axId val="786984002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="169839447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="786984002"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="786984002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="169839447"/>
+      </c:valAx>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Automation coverage'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Automation coverage'!$A$2:$A$19</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Automation coverage'!$E$2:$E$19</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1323558144"/>
+        <c:axId val="817590187"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1323558144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="817590187"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="817590187"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1323558144"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -1283,11 +1662,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1219572930"/>
-        <c:axId val="1181936063"/>
+        <c:axId val="1629492978"/>
+        <c:axId val="1582859452"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1219572930"/>
+        <c:axId val="1629492978"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,6 +1694,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -1332,10 +1712,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1181936063"/>
+        <c:crossAx val="1582859452"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1181936063"/>
+        <c:axId val="1582859452"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,7 +1784,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219572930"/>
+        <c:crossAx val="1629492978"/>
       </c:valAx>
       <c:lineChart>
         <c:varyColors val="0"/>
@@ -1420,6 +1800,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -1448,16 +1829,17 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="553369681"/>
-        <c:axId val="1221242671"/>
+        <c:axId val="309516070"/>
+        <c:axId val="1107777487"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="553369681"/>
+        <c:axId val="309516070"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
@@ -1475,10 +1857,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1221242671"/>
+        <c:crossAx val="1107777487"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1221242671"/>
+        <c:axId val="1107777487"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,7 +1929,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553369681"/>
+        <c:crossAx val="309516070"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -2513,10 +2895,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
@@ -2540,10 +2922,40 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 12" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -3070,249 +3482,225 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="27.0"/>
+    <col customWidth="1" min="2" max="2" width="10.14"/>
     <col customWidth="1" min="3" max="3" width="12.57"/>
     <col customWidth="1" min="4" max="4" width="13.14"/>
     <col customWidth="1" min="5" max="5" width="12.57"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="33"/>
-      <c r="B1" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35">
-        <f t="shared" ref="C2:C11" si="2">(1-(G2/E2))</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="35">
-        <f t="shared" ref="D2:D11" si="3">F2/(E2-G2)</f>
-        <v>0.99</v>
-      </c>
-      <c r="E2" s="36">
-        <f t="shared" ref="E2:G2" si="1">sum(E3:E12)</f>
-        <v>300</v>
-      </c>
-      <c r="F2" s="36">
+      <c r="A2" s="21">
+        <v>43990.0</v>
+      </c>
+      <c r="B2" s="26">
+        <v>98.0</v>
+      </c>
+      <c r="C2" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="24">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="23">
+        <f t="shared" ref="E2:E6" si="1">B2/sum(B2:D2)</f>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="21">
+        <v>43984.0</v>
+      </c>
+      <c r="B3" s="24">
+        <v>70.0</v>
+      </c>
+      <c r="C3" s="24">
+        <v>10.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="23">
         <f t="shared" si="1"/>
-        <v>297</v>
-      </c>
-      <c r="G2" s="36">
+        <v>0.8641975309</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="21">
+        <v>43976.0</v>
+      </c>
+      <c r="B4" s="24">
+        <v>30.0</v>
+      </c>
+      <c r="C4" s="24">
+        <v>30.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="39">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D3" s="39">
-        <f t="shared" si="3"/>
-        <v>0.99</v>
-      </c>
-      <c r="E3" s="36">
-        <v>100.0</v>
-      </c>
-      <c r="F3" s="36">
-        <v>99.0</v>
-      </c>
-      <c r="G3" s="36">
-        <v>0.0</v>
-      </c>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D4" s="39" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
+        <v>0.4918032787</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
     </row>
     <row r="5">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D5" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
+      <c r="A5" s="21">
+        <v>43970.0</v>
+      </c>
+      <c r="B5" s="24">
+        <v>10.0</v>
+      </c>
+      <c r="C5" s="24">
+        <v>50.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="1"/>
+        <v>0.1639344262</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D6" s="39" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
+      <c r="A6" s="21">
+        <v>43963.0</v>
+      </c>
+      <c r="B6" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="1"/>
+        <v>0.01923076923</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="39">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="39">
-        <f t="shared" si="3"/>
-        <v>0.99</v>
-      </c>
-      <c r="E7" s="36">
-        <v>100.0</v>
-      </c>
-      <c r="F7" s="36">
-        <v>99.0</v>
-      </c>
-      <c r="G7" s="36">
-        <v>0.0</v>
-      </c>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="34"/>
-      <c r="C8" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9">
-      <c r="A9" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D9" s="39">
-        <f t="shared" si="3"/>
-        <v>0.99</v>
-      </c>
-      <c r="E9" s="36">
-        <v>100.0</v>
-      </c>
-      <c r="F9" s="36">
-        <v>99.0</v>
-      </c>
-      <c r="G9" s="36">
-        <v>0.0</v>
-      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="34"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="39" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="41" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="41" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12">
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13">
-      <c r="C13" s="18" t="s">
-        <v>34</v>
-      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14">
-      <c r="C14" s="18" t="s">
-        <v>35</v>
-      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16">
+      <c r="I16" s="4"/>
     </row>
     <row r="21">
       <c r="A21" s="15"/>
@@ -3329,19 +3717,11 @@
       <c r="D22" s="17"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="R22" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="L22" s="19"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
     </row>
     <row r="23">
       <c r="A23" s="16"/>
@@ -3350,147 +3730,72 @@
       <c r="D23" s="17"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
-      <c r="N23" s="21">
-        <v>43963.0</v>
-      </c>
-      <c r="O23" s="22">
-        <v>1277.0</v>
-      </c>
-      <c r="P23" s="2">
-        <v>138.0</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>18.0</v>
-      </c>
-      <c r="R23" s="23">
-        <f t="shared" ref="R23:R30" si="4">O23/sum(O23:Q23)</f>
-        <v>0.8911374738</v>
-      </c>
+      <c r="L23" s="21"/>
+      <c r="M23" s="22"/>
+      <c r="P23" s="23"/>
     </row>
     <row r="24">
       <c r="A24" s="13"/>
       <c r="F24" s="18"/>
-      <c r="N24" s="21">
-        <v>43970.0</v>
-      </c>
-      <c r="O24" s="24">
-        <v>1295.0</v>
-      </c>
-      <c r="P24" s="24">
-        <v>155.0</v>
-      </c>
-      <c r="Q24" s="24">
-        <v>17.0</v>
-      </c>
-      <c r="R24" s="23">
-        <f t="shared" si="4"/>
-        <v>0.8827539196</v>
-      </c>
+      <c r="L24" s="21"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+      <c r="P24" s="23"/>
     </row>
     <row r="25">
-      <c r="N25" s="21">
-        <v>43976.0</v>
-      </c>
-      <c r="O25" s="24">
-        <v>1301.0</v>
-      </c>
-      <c r="P25" s="24">
-        <v>152.0</v>
-      </c>
-      <c r="Q25" s="24">
-        <v>17.0</v>
-      </c>
-      <c r="R25" s="23">
-        <f t="shared" si="4"/>
-        <v>0.8850340136</v>
-      </c>
+      <c r="L25" s="21"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="P25" s="23"/>
     </row>
     <row r="26">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
-      <c r="N26" s="21">
-        <v>43984.0</v>
-      </c>
-      <c r="O26" s="24">
-        <v>1322.0</v>
-      </c>
-      <c r="P26" s="24">
-        <v>125.0</v>
-      </c>
-      <c r="Q26" s="24">
-        <v>18.0</v>
-      </c>
-      <c r="R26" s="23">
-        <f t="shared" si="4"/>
-        <v>0.9023890785</v>
-      </c>
+      <c r="L26" s="21"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="P26" s="23"/>
     </row>
     <row r="27">
       <c r="A27" s="25"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="N27" s="21">
-        <v>43990.0</v>
-      </c>
-      <c r="O27" s="26">
-        <v>1340.0</v>
-      </c>
-      <c r="P27" s="26">
-        <v>116.0</v>
-      </c>
-      <c r="Q27" s="24">
-        <v>18.0</v>
-      </c>
-      <c r="R27" s="23">
-        <f t="shared" si="4"/>
-        <v>0.9090909091</v>
-      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="23"/>
     </row>
     <row r="28">
       <c r="A28" s="25"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="N28" s="21">
-        <v>43998.0</v>
-      </c>
-      <c r="R28" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="L28" s="21"/>
+      <c r="P28" s="23"/>
     </row>
     <row r="29">
       <c r="A29" s="20"/>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
-      <c r="N29" s="21">
-        <v>44005.0</v>
-      </c>
+      <c r="L29" s="21"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
       <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="P29" s="23"/>
     </row>
     <row r="30">
       <c r="A30" s="27"/>
       <c r="B30" s="28"/>
-      <c r="N30" s="21">
-        <v>44012.0</v>
-      </c>
+      <c r="L30" s="21"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
       <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="P30" s="23"/>
     </row>
     <row r="43">
       <c r="A43" s="29"/>
@@ -3504,7 +3809,7 @@
       <c r="I43" s="29"/>
     </row>
     <row r="44">
-      <c r="A44" s="44"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
@@ -3537,6 +3842,474 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="27.0"/>
+    <col customWidth="1" min="3" max="3" width="12.57"/>
+    <col customWidth="1" min="4" max="4" width="13.14"/>
+    <col customWidth="1" min="5" max="5" width="12.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35">
+        <f t="shared" ref="C2:C11" si="2">(1-(G2/E2))</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="35">
+        <f t="shared" ref="D2:D11" si="3">F2/(E2-G2)</f>
+        <v>0.99</v>
+      </c>
+      <c r="E2" s="36">
+        <f t="shared" ref="E2:G2" si="1">sum(E3:E12)</f>
+        <v>300</v>
+      </c>
+      <c r="F2" s="36">
+        <f t="shared" si="1"/>
+        <v>297</v>
+      </c>
+      <c r="G2" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D3" s="39">
+        <f t="shared" si="3"/>
+        <v>0.99</v>
+      </c>
+      <c r="E3" s="36">
+        <v>100.0</v>
+      </c>
+      <c r="F3" s="36">
+        <v>99.0</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D4" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="41" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D5" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D6" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="39">
+        <f t="shared" si="3"/>
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="36">
+        <v>100.0</v>
+      </c>
+      <c r="F7" s="36">
+        <v>99.0</v>
+      </c>
+      <c r="G7" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="34"/>
+      <c r="C8" s="41" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="39">
+        <f t="shared" si="3"/>
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="36">
+        <v>100.0</v>
+      </c>
+      <c r="F9" s="36">
+        <v>99.0</v>
+      </c>
+      <c r="G9" s="36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="34"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" s="39" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="41" t="str">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" s="41" t="str">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13">
+      <c r="C13" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="N23" s="21">
+        <v>43963.0</v>
+      </c>
+      <c r="O23" s="22">
+        <v>1277.0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>138.0</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>18.0</v>
+      </c>
+      <c r="R23" s="23">
+        <f t="shared" ref="R23:R30" si="4">O23/sum(O23:Q23)</f>
+        <v>0.8911374738</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="13"/>
+      <c r="F24" s="18"/>
+      <c r="N24" s="21">
+        <v>43970.0</v>
+      </c>
+      <c r="O24" s="24">
+        <v>1295.0</v>
+      </c>
+      <c r="P24" s="24">
+        <v>155.0</v>
+      </c>
+      <c r="Q24" s="24">
+        <v>17.0</v>
+      </c>
+      <c r="R24" s="23">
+        <f t="shared" si="4"/>
+        <v>0.8827539196</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="N25" s="21">
+        <v>43976.0</v>
+      </c>
+      <c r="O25" s="24">
+        <v>1301.0</v>
+      </c>
+      <c r="P25" s="24">
+        <v>152.0</v>
+      </c>
+      <c r="Q25" s="24">
+        <v>17.0</v>
+      </c>
+      <c r="R25" s="23">
+        <f t="shared" si="4"/>
+        <v>0.8850340136</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="N26" s="21">
+        <v>43984.0</v>
+      </c>
+      <c r="O26" s="24">
+        <v>1322.0</v>
+      </c>
+      <c r="P26" s="24">
+        <v>125.0</v>
+      </c>
+      <c r="Q26" s="24">
+        <v>18.0</v>
+      </c>
+      <c r="R26" s="23">
+        <f t="shared" si="4"/>
+        <v>0.9023890785</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="25"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="N27" s="21">
+        <v>43990.0</v>
+      </c>
+      <c r="O27" s="26">
+        <v>1340.0</v>
+      </c>
+      <c r="P27" s="26">
+        <v>116.0</v>
+      </c>
+      <c r="Q27" s="24">
+        <v>18.0</v>
+      </c>
+      <c r="R27" s="23">
+        <f t="shared" si="4"/>
+        <v>0.9090909091</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="25"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="N28" s="21">
+        <v>43998.0</v>
+      </c>
+      <c r="R28" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="20"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="N29" s="21">
+        <v>44005.0</v>
+      </c>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="N30" s="21">
+        <v>44012.0</v>
+      </c>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="44"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="32"/>
+    </row>
+    <row r="45">
+      <c r="I45" s="18"/>
+    </row>
+    <row r="46">
+      <c r="H46" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B30:D30"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="45" t="s">
@@ -3910,18 +4683,18 @@
   <mergeCells count="996">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
@@ -4235,22 +5008,22 @@
     <mergeCell ref="B325:C325"/>
     <mergeCell ref="B326:C326"/>
     <mergeCell ref="B327:C327"/>
-    <mergeCell ref="B671:C671"/>
-    <mergeCell ref="B672:C672"/>
-    <mergeCell ref="B673:C673"/>
-    <mergeCell ref="B674:C674"/>
-    <mergeCell ref="B675:C675"/>
-    <mergeCell ref="B676:C676"/>
-    <mergeCell ref="B677:C677"/>
-    <mergeCell ref="B678:C678"/>
-    <mergeCell ref="B679:C679"/>
-    <mergeCell ref="B680:C680"/>
-    <mergeCell ref="B681:C681"/>
-    <mergeCell ref="B682:C682"/>
-    <mergeCell ref="B683:C683"/>
-    <mergeCell ref="B684:C684"/>
-    <mergeCell ref="B685:C685"/>
-    <mergeCell ref="B686:C686"/>
+    <mergeCell ref="B328:C328"/>
+    <mergeCell ref="B329:C329"/>
+    <mergeCell ref="B330:C330"/>
+    <mergeCell ref="B331:C331"/>
+    <mergeCell ref="B332:C332"/>
+    <mergeCell ref="B333:C333"/>
+    <mergeCell ref="B334:C334"/>
+    <mergeCell ref="B335:C335"/>
+    <mergeCell ref="B336:C336"/>
+    <mergeCell ref="B337:C337"/>
+    <mergeCell ref="B338:C338"/>
+    <mergeCell ref="B339:C339"/>
+    <mergeCell ref="B340:C340"/>
+    <mergeCell ref="B341:C341"/>
+    <mergeCell ref="B342:C342"/>
+    <mergeCell ref="B343:C343"/>
     <mergeCell ref="B687:C687"/>
     <mergeCell ref="B688:C688"/>
     <mergeCell ref="B689:C689"/>
@@ -4480,38 +5253,6 @@
     <mergeCell ref="B913:C913"/>
     <mergeCell ref="B914:C914"/>
     <mergeCell ref="B915:C915"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B968:C968"/>
-    <mergeCell ref="B969:C969"/>
-    <mergeCell ref="B970:C970"/>
-    <mergeCell ref="B971:C971"/>
-    <mergeCell ref="B972:C972"/>
-    <mergeCell ref="B973:C973"/>
-    <mergeCell ref="B974:C974"/>
-    <mergeCell ref="B975:C975"/>
-    <mergeCell ref="B976:C976"/>
-    <mergeCell ref="B977:C977"/>
-    <mergeCell ref="B978:C978"/>
-    <mergeCell ref="B979:C979"/>
-    <mergeCell ref="B980:C980"/>
-    <mergeCell ref="B981:C981"/>
-    <mergeCell ref="B982:C982"/>
-    <mergeCell ref="B983:C983"/>
-    <mergeCell ref="B984:C984"/>
-    <mergeCell ref="B985:C985"/>
-    <mergeCell ref="B993:C993"/>
-    <mergeCell ref="B994:C994"/>
-    <mergeCell ref="B995:C995"/>
-    <mergeCell ref="B996:C996"/>
-    <mergeCell ref="B986:C986"/>
-    <mergeCell ref="B987:C987"/>
-    <mergeCell ref="B988:C988"/>
-    <mergeCell ref="B989:C989"/>
-    <mergeCell ref="B990:C990"/>
-    <mergeCell ref="B991:C991"/>
-    <mergeCell ref="B992:C992"/>
     <mergeCell ref="B916:C916"/>
     <mergeCell ref="B917:C917"/>
     <mergeCell ref="B918:C918"/>
@@ -4528,6 +5269,22 @@
     <mergeCell ref="B929:C929"/>
     <mergeCell ref="B930:C930"/>
     <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B981:C981"/>
+    <mergeCell ref="B982:C982"/>
+    <mergeCell ref="B983:C983"/>
+    <mergeCell ref="B984:C984"/>
+    <mergeCell ref="B985:C985"/>
+    <mergeCell ref="B986:C986"/>
+    <mergeCell ref="B987:C987"/>
+    <mergeCell ref="B995:C995"/>
+    <mergeCell ref="B996:C996"/>
+    <mergeCell ref="B988:C988"/>
+    <mergeCell ref="B989:C989"/>
+    <mergeCell ref="B990:C990"/>
+    <mergeCell ref="B991:C991"/>
+    <mergeCell ref="B992:C992"/>
+    <mergeCell ref="B993:C993"/>
+    <mergeCell ref="B994:C994"/>
     <mergeCell ref="B932:C932"/>
     <mergeCell ref="B933:C933"/>
     <mergeCell ref="B934:C934"/>
@@ -4561,22 +5318,22 @@
     <mergeCell ref="B962:C962"/>
     <mergeCell ref="B963:C963"/>
     <mergeCell ref="B964:C964"/>
-    <mergeCell ref="B328:C328"/>
-    <mergeCell ref="B329:C329"/>
-    <mergeCell ref="B330:C330"/>
-    <mergeCell ref="B331:C331"/>
-    <mergeCell ref="B332:C332"/>
-    <mergeCell ref="B333:C333"/>
-    <mergeCell ref="B334:C334"/>
-    <mergeCell ref="B335:C335"/>
-    <mergeCell ref="B336:C336"/>
-    <mergeCell ref="B337:C337"/>
-    <mergeCell ref="B338:C338"/>
-    <mergeCell ref="B339:C339"/>
-    <mergeCell ref="B340:C340"/>
-    <mergeCell ref="B341:C341"/>
-    <mergeCell ref="B342:C342"/>
-    <mergeCell ref="B343:C343"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B968:C968"/>
+    <mergeCell ref="B969:C969"/>
+    <mergeCell ref="B970:C970"/>
+    <mergeCell ref="B971:C971"/>
+    <mergeCell ref="B972:C972"/>
+    <mergeCell ref="B973:C973"/>
+    <mergeCell ref="B974:C974"/>
+    <mergeCell ref="B975:C975"/>
+    <mergeCell ref="B976:C976"/>
+    <mergeCell ref="B977:C977"/>
+    <mergeCell ref="B978:C978"/>
+    <mergeCell ref="B979:C979"/>
+    <mergeCell ref="B980:C980"/>
     <mergeCell ref="B344:C344"/>
     <mergeCell ref="B345:C345"/>
     <mergeCell ref="B346:C346"/>
@@ -4904,12 +5661,28 @@
     <mergeCell ref="B668:C668"/>
     <mergeCell ref="B669:C669"/>
     <mergeCell ref="B670:C670"/>
+    <mergeCell ref="B671:C671"/>
+    <mergeCell ref="B672:C672"/>
+    <mergeCell ref="B673:C673"/>
+    <mergeCell ref="B674:C674"/>
+    <mergeCell ref="B675:C675"/>
+    <mergeCell ref="B676:C676"/>
+    <mergeCell ref="B677:C677"/>
+    <mergeCell ref="B678:C678"/>
+    <mergeCell ref="B679:C679"/>
+    <mergeCell ref="B680:C680"/>
+    <mergeCell ref="B681:C681"/>
+    <mergeCell ref="B682:C682"/>
+    <mergeCell ref="B683:C683"/>
+    <mergeCell ref="B684:C684"/>
+    <mergeCell ref="B685:C685"/>
+    <mergeCell ref="B686:C686"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>